<commit_message>
Pb de contrast régler
</commit_message>
<xml_diff>
--- a/P4_Audit.xlsx
+++ b/P4_Audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\Berri_Sarah_4_092022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE750691-8F4F-462A-B1C9-4B77C819B5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80176A05-BBFB-406C-8C94-104AE6CC55C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055226-pensez-mobile-first</t>
   </si>
   <si>
-    <t>Avoir peu de liens mais de façon efficace et intelligente   Supprimer les liens qui n'ont pas de rapport avec le thème</t>
-  </si>
-  <si>
     <t>Couleurs et textes</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
   </si>
   <si>
     <t>Contenu</t>
-  </si>
-  <si>
-    <t>Le site est bien responsive</t>
   </si>
   <si>
     <t>Le formulaire est clair, et les labels ont été complétés</t>
@@ -222,9 +216,6 @@
     </r>
   </si>
   <si>
-    <t>Minification JS</t>
-  </si>
-  <si>
     <t>Les fichiers JS requis ont été minifier afin de réduire le temps de chargement des pages</t>
   </si>
   <si>
@@ -232,6 +223,15 @@
   </si>
   <si>
     <t>Renommer l'URL de la page contact                            Renommer les balises lang et title                                                                                   Ajouter une description d'images dans les attributs alt et non une répétition de mots                                                                     Ajout des balises méta keywords, description, et robots                                  Enlever l'image en tant que texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minification des fichiers JavaScript </t>
+  </si>
+  <si>
+    <t>Avoir peu de liens mais de façon efficace et intelligente / Supprimer les liens qui n'ont pas de rapport avec le thème</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le site est bien responsive, le chargement </t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,15 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
@@ -411,17 +402,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -641,17 +644,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="28.08984375" customWidth="1"/>
-    <col min="3" max="3" width="47.26953125" customWidth="1"/>
-    <col min="4" max="4" width="53.1796875" customWidth="1"/>
-    <col min="5" max="5" width="40.1796875" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.1796875" customWidth="1"/>
+    <col min="4" max="4" width="65.08984375" customWidth="1"/>
+    <col min="5" max="5" width="65" customWidth="1"/>
     <col min="6" max="6" width="91.453125" customWidth="1"/>
     <col min="7" max="26" width="10.54296875" customWidth="1"/>
   </cols>
@@ -696,223 +699,223 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" s="17" customFormat="1" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:26" s="14" customFormat="1" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:26" s="17" customFormat="1" ht="241.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" s="14" customFormat="1" ht="241.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:26" s="14" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:26" s="14" customFormat="1" ht="172.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:26" s="14" customFormat="1" ht="109.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:26" s="14" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:26" s="14" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:26" s="14" customFormat="1" ht="115.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="E9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:26" s="14" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:26" s="17" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:26" s="17" customFormat="1" ht="172.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:26" s="17" customFormat="1" ht="109.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:26" s="17" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:26" s="17" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:26" s="17" customFormat="1" ht="115.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:26" s="17" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:26" s="17" customFormat="1" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:26" s="14" customFormat="1" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>23</v>
       </c>
@@ -920,81 +923,81 @@
         <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:26" s="17" customFormat="1" ht="158.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:26" s="14" customFormat="1" ht="158.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:26" s="17" customFormat="1" ht="172.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:26" s="14" customFormat="1" ht="172.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>32</v>
-      </c>
       <c r="E13" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:26" s="17" customFormat="1" ht="158.4" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:26" s="14" customFormat="1" ht="158.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>

</xml_diff>

<commit_message>
maj audit et dossier
</commit_message>
<xml_diff>
--- a/P4_Audit.xlsx
+++ b/P4_Audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\Berri_Sarah_4_092022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80176A05-BBFB-406C-8C94-104AE6CC55C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A5A053-8D7A-416E-8AD8-194A13C960E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>Formulaire</t>
   </si>
   <si>
-    <t>Le formulaire est accessible mais des modifications doivent y être apportées notamment les labels, il faudrait également modifier le design du formulaire</t>
-  </si>
-  <si>
     <t>Le formulaire doit être améliorer, modifier le style des champs de saisies</t>
   </si>
   <si>
@@ -148,15 +145,6 @@
   </si>
   <si>
     <t>Le formulaire est clair, et les labels ont été complétés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Augmentez la taille des textes Et leur couleur afin d'avoir une cohérence entre les deux </t>
-  </si>
-  <si>
-    <t>Les textes ont été agrandit et la couleur des texte a été modifier</t>
-  </si>
-  <si>
-    <t>https://rgaa.tanaguru.com/rgaa3-criteres.html#test-3-3-1</t>
   </si>
   <si>
     <t>Balise méta = "keywords"</t>
@@ -232,6 +220,29 @@
   </si>
   <si>
     <t xml:space="preserve">Le site est bien responsive, le chargement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le formulaire est accessible mais des modifications doivent y être apportées notamment les labels, il faudrait également modifier le design du formulaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augmentez la taille des textes, et régler les problèmes de contrast afin d'avoir une cohérence entre les deux </t>
+  </si>
+  <si>
+    <t>Les textes ont été agrandit et la couleur des texte a été modifier, le contrast est correct</t>
+  </si>
+  <si>
+    <r>
+      <t>https://rgaa.tanaguru.com/rgaa3-criteres.html#test-3-3-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -644,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J12" sqref="I12:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -731,13 +742,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>12</v>
@@ -755,13 +766,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>13</v>
@@ -785,10 +796,10 @@
         <v>17</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -800,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>14</v>
@@ -809,10 +820,10 @@
         <v>15</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -827,16 +838,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -851,16 +862,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -872,19 +883,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>48</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -896,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>19</v>
@@ -905,10 +916,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -926,10 +937,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>24</v>
@@ -950,13 +961,13 @@
         <v>27</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -971,16 +982,16 @@
         <v>29</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -3343,11 +3354,11 @@
     <hyperlink ref="F5" r:id="rId4" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist" xr:uid="{311DBCEE-4994-43A2-8F5E-FD49EDBD3E73}"/>
     <hyperlink ref="F6" r:id="rId5" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist" xr:uid="{FAFE0CED-F9D7-43C2-B97B-3690F51E85EC}"/>
     <hyperlink ref="F11" r:id="rId6" location="test-3-3-1" xr:uid="{71AF6E9A-7110-40D0-BD74-4C06CD18622B}"/>
-    <hyperlink ref="F12" r:id="rId7" location="test-3-3-1" xr:uid="{108DEA9F-3B87-4B77-A18D-93C44FC06499}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{467C0A8A-05E2-4170-A2D6-6065357EAC1C}"/>
-    <hyperlink ref="F13" r:id="rId9" xr:uid="{6FF4161A-9EF9-4E2A-B228-DE53217FE978}"/>
-    <hyperlink ref="F10" r:id="rId10" xr:uid="{6BAD20B1-685A-40E4-BE86-3F920428288B}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{B47C802B-A761-4E3E-A99A-28D370CB3D6D}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{467C0A8A-05E2-4170-A2D6-6065357EAC1C}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{6FF4161A-9EF9-4E2A-B228-DE53217FE978}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{6BAD20B1-685A-40E4-BE86-3F920428288B}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{B47C802B-A761-4E3E-A99A-28D370CB3D6D}"/>
+    <hyperlink ref="F12" r:id="rId11" location="test-3-3-1" display="https://rgaa.tanaguru.com/rgaa3-criteres.html#test-3-3-1" xr:uid="{108DEA9F-3B87-4B77-A18D-93C44FC06499}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId12"/>

</xml_diff>